<commit_message>
50 rbi/ms productive sheet collection
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/4475-RBI-ACTCTR-MEET-WEEKLYonFRI-ACTGRP-ACTCLIENT-DISJLG02JAN-COLLSHEETON25DEC2014.xlsx
+++ b/Mifos Automation Excels/Client/4475-RBI-ACTCTR-MEET-WEEKLYonFRI-ACTGRP-ACTCLIENT-DISJLG02JAN-COLLSHEETON25DEC2014.xlsx
@@ -242,9 +242,6 @@
     <t>Grou4475</t>
   </si>
   <si>
-    <t>Collection sheet cannot be generated for center/group without attach meeting define</t>
-  </si>
-  <si>
     <t>clickonmorebutton</t>
   </si>
   <si>
@@ -261,6 +258,9 @@
   </si>
   <si>
     <t>selectweekdaysfriday</t>
+  </si>
+  <si>
+    <t>Selected calendar date is not a valid recurrence date</t>
   </si>
 </sst>
 </file>
@@ -289,7 +289,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="Arial Unicode MS"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -409,9 +409,11 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,7 +778,7 @@
     </row>
     <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -784,15 +786,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B8" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" s="20" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" s="5">
         <v>42005</v>
@@ -800,17 +802,17 @@
     </row>
     <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>77</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -936,7 +938,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -996,12 +998,13 @@
       <c r="A7" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>73</v>
+      <c r="B7" s="22" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>